<commit_message>
no data for Disciplinary Actions 2003
</commit_message>
<xml_diff>
--- a/ope.ed.gov/2003/criminal-offenses-on-campus-student-housing-facilities-virginia-colleges-and-universities-crime-2003.xlsx
+++ b/ope.ed.gov/2003/criminal-offenses-on-campus-student-housing-facilities-virginia-colleges-and-universities-crime-2003.xlsx
@@ -13,16 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Criminal Offenses - On-campus Student Housing Facilities</t>
-  </si>
-  <si>
-    <t>Survey year</t>
-  </si>
-  <si>
-    <t>Unitid</t>
-  </si>
-  <si>
-    <t>Institution name</t>
+    <t>Survey Year</t>
+  </si>
+  <si>
+    <t>UnitID</t>
+  </si>
+  <si>
+    <t>Institution Name</t>
   </si>
   <si>
     <t>Campus ID</t>
@@ -34,28 +31,28 @@
     <t>Institution Size</t>
   </si>
   <si>
-    <t>Murder/Non-negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible</t>
+    <t>Murder/Non-Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible</t>
   </si>
   <si>
     <t>Robbery</t>
   </si>
   <si>
-    <t>Aggravated assault</t>
+    <t>Aggravated Assault</t>
   </si>
   <si>
     <t>Burglary</t>
   </si>
   <si>
-    <t>Motor vehicle theft</t>
+    <t>Motor Vehicle Theft</t>
   </si>
   <si>
     <t>Arson</t>
@@ -445,52 +442,94 @@
       <c t="s" s="1" r="A1">
         <v>0</v>
       </c>
+      <c t="s" s="1" r="B1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>4</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="J1">
+        <v>9</v>
+      </c>
+      <c t="s" s="1" r="K1">
+        <v>10</v>
+      </c>
+      <c t="s" s="1" r="L1">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="M1">
+        <v>12</v>
+      </c>
+      <c t="s" s="1" r="N1">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="O1">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>1</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>2</v>
+      <c s="1" r="A2">
+        <v>2003.0</v>
+      </c>
+      <c s="1" r="B2">
+        <v>231420.0</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>3</v>
-      </c>
-      <c t="s" s="1" r="D2">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c s="1" r="D2">
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>5</v>
-      </c>
-      <c t="s" s="1" r="F2">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="G2">
-        <v>7</v>
-      </c>
-      <c t="s" s="1" r="H2">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="I2">
-        <v>9</v>
-      </c>
-      <c t="s" s="1" r="J2">
-        <v>10</v>
-      </c>
-      <c t="s" s="1" r="K2">
-        <v>11</v>
-      </c>
-      <c t="s" s="1" r="L2">
-        <v>12</v>
-      </c>
-      <c t="s" s="1" r="M2">
-        <v>13</v>
-      </c>
-      <c t="s" s="1" r="N2">
-        <v>14</v>
-      </c>
-      <c t="s" s="1" r="O2">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c s="1" r="F2">
+        <v>2849.0</v>
+      </c>
+      <c s="1" r="G2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="I2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="J2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="K2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="L2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="M2">
+        <v>4.0</v>
+      </c>
+      <c s="1" r="N2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="O2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -498,19 +537,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B3">
-        <v>231420.0</v>
+        <v>366793.0</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c s="1" r="D3">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c s="1" r="F3">
-        <v>2849.0</v>
+        <v>204.0</v>
       </c>
       <c s="1" r="G3">
         <v>0.0</v>
@@ -531,7 +570,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M3">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N3">
         <v>0.0</v>
@@ -545,19 +584,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B4">
-        <v>366793.0</v>
+        <v>231554.0</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c s="1" r="D4">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="1" r="F4">
-        <v>204.0</v>
+        <v>731.0</v>
       </c>
       <c s="1" r="G4">
         <v>0.0</v>
@@ -592,19 +631,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B5">
-        <v>231554.0</v>
+        <v>231581.0</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c s="1" r="D5">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c s="1" r="F5">
-        <v>731.0</v>
+        <v>1403.0</v>
       </c>
       <c s="1" r="G5">
         <v>0.0</v>
@@ -613,7 +652,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I5">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J5">
         <v>0.0</v>
@@ -625,7 +664,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M5">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="N5">
         <v>0.0</v>
@@ -639,19 +678,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B6">
-        <v>231581.0</v>
+        <v>231712.0</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c s="1" r="D6">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c s="1" r="F6">
-        <v>1403.0</v>
+        <v>4812.0</v>
       </c>
       <c s="1" r="G6">
         <v>0.0</v>
@@ -660,7 +699,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I6">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J6">
         <v>0.0</v>
@@ -686,19 +725,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B7">
-        <v>231712.0</v>
+        <v>231624.0</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c s="1" r="D7">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c s="1" r="F7">
-        <v>4812.0</v>
+        <v>7749.0</v>
       </c>
       <c s="1" r="G7">
         <v>0.0</v>
@@ -733,19 +772,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B8">
-        <v>231624.0</v>
+        <v>232043.0</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c s="1" r="D8">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c s="1" r="F8">
-        <v>7749.0</v>
+        <v>1245.0</v>
       </c>
       <c s="1" r="G8">
         <v>0.0</v>
@@ -754,7 +793,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J8">
         <v>0.0</v>
@@ -766,7 +805,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M8">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N8">
         <v>0.0</v>
@@ -780,19 +819,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B9">
-        <v>232043.0</v>
+        <v>232025.0</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c s="1" r="D9">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E9">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c s="1" r="F9">
-        <v>1245.0</v>
+        <v>927.0</v>
       </c>
       <c s="1" r="G9">
         <v>0.0</v>
@@ -813,7 +852,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M9">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="N9">
         <v>0.0</v>
@@ -827,19 +866,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B10">
-        <v>232025.0</v>
+        <v>232089.0</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c s="1" r="D10">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E10">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c s="1" r="F10">
-        <v>927.0</v>
+        <v>954.0</v>
       </c>
       <c s="1" r="G10">
         <v>0.0</v>
@@ -848,7 +887,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I10">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J10">
         <v>0.0</v>
@@ -860,13 +899,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M10">
-        <v>5.0</v>
+        <v>28.0</v>
       </c>
       <c s="1" r="N10">
         <v>0.0</v>
       </c>
       <c s="1" r="O10">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="11">
@@ -874,19 +913,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B11">
-        <v>232089.0</v>
+        <v>232186.0</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c s="1" r="D11">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E11">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c s="1" r="F11">
-        <v>954.0</v>
+        <v>28246.0</v>
       </c>
       <c s="1" r="G11">
         <v>0.0</v>
@@ -895,25 +934,25 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I11">
+        <v>13.0</v>
+      </c>
+      <c s="1" r="J11">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="K11">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="L11">
+        <v>1.0</v>
+      </c>
+      <c s="1" r="M11">
+        <v>10.0</v>
+      </c>
+      <c s="1" r="N11">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="O11">
         <v>2.0</v>
-      </c>
-      <c s="1" r="J11">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="K11">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="L11">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="M11">
-        <v>28.0</v>
-      </c>
-      <c s="1" r="N11">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="O11">
-        <v>6.0</v>
       </c>
     </row>
     <row r="12">
@@ -921,19 +960,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B12">
-        <v>232186.0</v>
+        <v>232256.0</v>
       </c>
       <c t="s" s="1" r="C12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c s="1" r="D12">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E12">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c s="1" r="F12">
-        <v>28246.0</v>
+        <v>1039.0</v>
       </c>
       <c s="1" r="G12">
         <v>0.0</v>
@@ -942,7 +981,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I12">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J12">
         <v>0.0</v>
@@ -951,16 +990,16 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L12">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M12">
-        <v>10.0</v>
+        <v>26.0</v>
       </c>
       <c s="1" r="N12">
         <v>0.0</v>
       </c>
       <c s="1" r="O12">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -968,19 +1007,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B13">
-        <v>232256.0</v>
+        <v>232265.0</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c s="1" r="D13">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E13">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c s="1" r="F13">
-        <v>1039.0</v>
+        <v>5797.0</v>
       </c>
       <c s="1" r="G13">
         <v>0.0</v>
@@ -989,7 +1028,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I13">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J13">
         <v>0.0</v>
@@ -1001,7 +1040,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M13">
-        <v>26.0</v>
+        <v>47.0</v>
       </c>
       <c s="1" r="N13">
         <v>0.0</v>
@@ -1015,19 +1054,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B14">
-        <v>232265.0</v>
+        <v>232308.0</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c s="1" r="D14">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E14">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c s="1" r="F14">
-        <v>5797.0</v>
+        <v>1090.0</v>
       </c>
       <c s="1" r="G14">
         <v>0.0</v>
@@ -1045,10 +1084,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L14">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M14">
-        <v>47.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="N14">
         <v>0.0</v>
@@ -1062,19 +1101,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B15">
-        <v>232308.0</v>
+        <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c s="1" r="D15">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E15">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c s="1" r="F15">
-        <v>1090.0</v>
+        <v>16203.0</v>
       </c>
       <c s="1" r="G15">
         <v>0.0</v>
@@ -1083,7 +1122,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I15">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J15">
         <v>0.0</v>
@@ -1095,7 +1134,7 @@
         <v>1.0</v>
       </c>
       <c s="1" r="M15">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c s="1" r="N15">
         <v>0.0</v>
@@ -1112,13 +1151,13 @@
         <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c s="1" r="D16">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c s="1" r="F16">
         <v>16203.0</v>
@@ -1130,7 +1169,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I16">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J16">
         <v>0.0</v>
@@ -1139,10 +1178,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L16">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M16">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N16">
         <v>0.0</v>
@@ -1159,13 +1198,13 @@
         <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c s="1" r="D17">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c t="s" s="1" r="E17">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c s="1" r="F17">
         <v>16203.0</v>
@@ -1203,19 +1242,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B18">
-        <v>232423.0</v>
+        <v>231837.0</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c s="1" r="D18">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E18">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c s="1" r="F18">
-        <v>16203.0</v>
+        <v>635.0</v>
       </c>
       <c s="1" r="G18">
         <v>0.0</v>
@@ -1250,19 +1289,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B19">
-        <v>231837.0</v>
+        <v>232469.0</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c s="1" r="D19">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E19">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c s="1" r="F19">
-        <v>635.0</v>
+        <v>831.0</v>
       </c>
       <c s="1" r="G19">
         <v>0.0</v>
@@ -1283,10 +1322,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M19">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N19">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="O19">
         <v>0.0</v>
@@ -1297,19 +1336,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B20">
-        <v>232469.0</v>
+        <v>232557.0</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c s="1" r="D20">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E20">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c s="1" r="F20">
-        <v>831.0</v>
+        <v>9050.0</v>
       </c>
       <c s="1" r="G20">
         <v>0.0</v>
@@ -1330,10 +1369,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M20">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c s="1" r="N20">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="O20">
         <v>0.0</v>
@@ -1344,19 +1383,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B21">
-        <v>232557.0</v>
+        <v>232566.0</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c s="1" r="D21">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E21">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c s="1" r="F21">
-        <v>9050.0</v>
+        <v>4252.0</v>
       </c>
       <c s="1" r="G21">
         <v>0.0</v>
@@ -1365,7 +1404,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I21">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="J21">
         <v>0.0</v>
@@ -1377,7 +1416,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M21">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N21">
         <v>0.0</v>
@@ -1391,19 +1430,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B22">
-        <v>232566.0</v>
+        <v>232609.0</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c s="1" r="D22">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c s="1" r="F22">
-        <v>4252.0</v>
+        <v>2009.0</v>
       </c>
       <c s="1" r="G22">
         <v>0.0</v>
@@ -1412,7 +1451,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I22">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J22">
         <v>0.0</v>
@@ -1421,7 +1460,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L22">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="M22">
         <v>1.0</v>
@@ -1438,19 +1477,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B23">
-        <v>232609.0</v>
+        <v>232618.0</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c s="1" r="D23">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E23">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c s="1" r="F23">
-        <v>2009.0</v>
+        <v>158.0</v>
       </c>
       <c s="1" r="G23">
         <v>0.0</v>
@@ -1459,7 +1498,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I23">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J23">
         <v>0.0</v>
@@ -1468,10 +1507,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L23">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M23">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N23">
         <v>0.0</v>
@@ -1485,19 +1524,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B24">
-        <v>232618.0</v>
+        <v>232672.0</v>
       </c>
       <c t="s" s="1" r="C24">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c s="1" r="D24">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E24">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c s="1" r="F24">
-        <v>158.0</v>
+        <v>1731.0</v>
       </c>
       <c s="1" r="G24">
         <v>0.0</v>
@@ -1506,7 +1545,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I24">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J24">
         <v>0.0</v>
@@ -1532,19 +1571,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B25">
-        <v>232672.0</v>
+        <v>232706.0</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c s="1" r="D25">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E25">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c s="1" r="F25">
-        <v>1731.0</v>
+        <v>3741.0</v>
       </c>
       <c s="1" r="G25">
         <v>0.0</v>
@@ -1553,7 +1592,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I25">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J25">
         <v>0.0</v>
@@ -1579,19 +1618,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B26">
-        <v>232706.0</v>
+        <v>232937.0</v>
       </c>
       <c t="s" s="1" r="C26">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c s="1" r="D26">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E26">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c s="1" r="F26">
-        <v>3741.0</v>
+        <v>6846.0</v>
       </c>
       <c s="1" r="G26">
         <v>0.0</v>
@@ -1600,7 +1639,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I26">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="J26">
         <v>0.0</v>
@@ -1612,13 +1651,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M26">
-        <v>0.0</v>
+        <v>38.0</v>
       </c>
       <c s="1" r="N26">
         <v>0.0</v>
       </c>
       <c s="1" r="O26">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="27">
@@ -1626,19 +1665,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B27">
-        <v>232937.0</v>
+        <v>232982.0</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c s="1" r="D27">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E27">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c s="1" r="F27">
-        <v>6846.0</v>
+        <v>20802.0</v>
       </c>
       <c s="1" r="G27">
         <v>0.0</v>
@@ -1647,25 +1686,25 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I27">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J27">
         <v>0.0</v>
       </c>
       <c s="1" r="K27">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="L27">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M27">
-        <v>38.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="N27">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="O27">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28">
@@ -1673,19 +1712,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B28">
-        <v>232982.0</v>
+        <v>233277.0</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c s="1" r="D28">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E28">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c s="1" r="F28">
-        <v>20802.0</v>
+        <v>9219.0</v>
       </c>
       <c s="1" r="G28">
         <v>0.0</v>
@@ -1694,22 +1733,22 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I28">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c s="1" r="J28">
         <v>0.0</v>
       </c>
       <c s="1" r="K28">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="L28">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="M28">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N28">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="O28">
         <v>0.0</v>
@@ -1720,19 +1759,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B29">
-        <v>233277.0</v>
+        <v>233301.0</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c s="1" r="D29">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E29">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c s="1" r="F29">
-        <v>9219.0</v>
+        <v>737.0</v>
       </c>
       <c s="1" r="G29">
         <v>0.0</v>
@@ -1741,7 +1780,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I29">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J29">
         <v>0.0</v>
@@ -1750,10 +1789,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L29">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M29">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N29">
         <v>0.0</v>
@@ -1767,19 +1806,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B30">
-        <v>233301.0</v>
+        <v>233295.0</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c s="1" r="D30">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E30">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c s="1" r="F30">
-        <v>737.0</v>
+        <v>1118.0</v>
       </c>
       <c s="1" r="G30">
         <v>0.0</v>
@@ -1797,10 +1836,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L30">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M30">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c s="1" r="N30">
         <v>0.0</v>
@@ -1814,19 +1853,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B31">
-        <v>233295.0</v>
+        <v>231651.0</v>
       </c>
       <c t="s" s="1" r="C31">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c s="1" r="D31">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E31">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c s="1" r="F31">
-        <v>1118.0</v>
+        <v>3173.0</v>
       </c>
       <c s="1" r="G31">
         <v>0.0</v>
@@ -1835,7 +1874,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I31">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J31">
         <v>0.0</v>
@@ -1844,10 +1883,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L31">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M31">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N31">
         <v>0.0</v>
@@ -1861,19 +1900,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B32">
-        <v>231651.0</v>
+        <v>233426.0</v>
       </c>
       <c t="s" s="1" r="C32">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c s="1" r="D32">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E32">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c s="1" r="F32">
-        <v>3173.0</v>
+        <v>1899.0</v>
       </c>
       <c s="1" r="G32">
         <v>0.0</v>
@@ -1882,7 +1921,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I32">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J32">
         <v>0.0</v>
@@ -1894,7 +1933,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M32">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c s="1" r="N32">
         <v>0.0</v>
@@ -1908,19 +1947,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B33">
-        <v>233426.0</v>
+        <v>233499.0</v>
       </c>
       <c t="s" s="1" r="C33">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c s="1" r="D33">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E33">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c s="1" r="F33">
-        <v>1899.0</v>
+        <v>475.0</v>
       </c>
       <c s="1" r="G33">
         <v>0.0</v>
@@ -1929,7 +1968,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I33">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J33">
         <v>0.0</v>
@@ -1938,10 +1977,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L33">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="M33">
-        <v>8.0</v>
+        <v>25.0</v>
       </c>
       <c s="1" r="N33">
         <v>0.0</v>
@@ -1955,19 +1994,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B34">
-        <v>233499.0</v>
+        <v>233541.0</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c s="1" r="D34">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E34">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c s="1" r="F34">
-        <v>475.0</v>
+        <v>2851.0</v>
       </c>
       <c s="1" r="G34">
         <v>0.0</v>
@@ -1985,10 +2024,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L34">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M34">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N34">
         <v>0.0</v>
@@ -2002,19 +2041,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B35">
-        <v>233541.0</v>
+        <v>233611.0</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c s="1" r="D35">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E35">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c s="1" r="F35">
-        <v>2851.0</v>
+        <v>579.0</v>
       </c>
       <c s="1" r="G35">
         <v>0.0</v>
@@ -2023,7 +2062,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I35">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J35">
         <v>0.0</v>
@@ -2032,7 +2071,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L35">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M35">
         <v>0.0</v>
@@ -2049,19 +2088,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B36">
-        <v>233611.0</v>
+        <v>233718.0</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c s="1" r="D36">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E36">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c s="1" r="F36">
-        <v>579.0</v>
+        <v>709.0</v>
       </c>
       <c s="1" r="G36">
         <v>0.0</v>
@@ -2070,7 +2109,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I36">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J36">
         <v>0.0</v>
@@ -2079,7 +2118,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L36">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M36">
         <v>0.0</v>
@@ -2096,19 +2135,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B37">
-        <v>233718.0</v>
+        <v>233897.0</v>
       </c>
       <c t="s" s="1" r="C37">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c s="1" r="D37">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E37">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c s="1" r="F37">
-        <v>709.0</v>
+        <v>1703.0</v>
       </c>
       <c s="1" r="G37">
         <v>0.0</v>
@@ -2129,7 +2168,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M37">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N37">
         <v>0.0</v>
@@ -2143,19 +2182,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B38">
-        <v>233897.0</v>
+        <v>233842.0</v>
       </c>
       <c t="s" s="1" r="C38">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c s="1" r="D38">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E38">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c s="1" r="F38">
-        <v>1703.0</v>
+        <v>384.0</v>
       </c>
       <c s="1" r="G38">
         <v>0.0</v>
@@ -2176,7 +2215,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M38">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N38">
         <v>0.0</v>
@@ -2193,13 +2232,13 @@
         <v>233842.0</v>
       </c>
       <c t="s" s="1" r="C39">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c s="1" r="D39">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E39">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c s="1" r="F39">
         <v>384.0</v>
@@ -2211,7 +2250,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J39">
         <v>0.0</v>
@@ -2223,7 +2262,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M39">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c s="1" r="N39">
         <v>0.0</v>
@@ -2237,19 +2276,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B40">
-        <v>233842.0</v>
+        <v>232681.0</v>
       </c>
       <c t="s" s="1" r="C40">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c s="1" r="D40">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E40">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c s="1" r="F40">
-        <v>384.0</v>
+        <v>4792.0</v>
       </c>
       <c s="1" r="G40">
         <v>0.0</v>
@@ -2270,13 +2309,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M40">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N40">
         <v>0.0</v>
       </c>
       <c s="1" r="O40">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="41">
@@ -2284,19 +2323,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B41">
-        <v>232681.0</v>
+        <v>233374.0</v>
       </c>
       <c t="s" s="1" r="C41">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c s="1" r="D41">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E41">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c s="1" r="F41">
-        <v>4792.0</v>
+        <v>4444.0</v>
       </c>
       <c s="1" r="G41">
         <v>0.0</v>
@@ -2305,7 +2344,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I41">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J41">
         <v>0.0</v>
@@ -2314,10 +2353,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L41">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M41">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="N41">
         <v>0.0</v>
@@ -2331,19 +2370,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B42">
-        <v>233374.0</v>
+        <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C42">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c s="1" r="D42">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E42">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c s="1" r="F42">
-        <v>4444.0</v>
+        <v>23077.0</v>
       </c>
       <c s="1" r="G42">
         <v>0.0</v>
@@ -2352,7 +2391,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I42">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="J42">
         <v>0.0</v>
@@ -2361,16 +2400,16 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L42">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M42">
-        <v>5.0</v>
+        <v>18.0</v>
       </c>
       <c s="1" r="N42">
         <v>0.0</v>
       </c>
       <c s="1" r="O42">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
@@ -2381,13 +2420,13 @@
         <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C43">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c s="1" r="D43">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c t="s" s="1" r="E43">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c s="1" r="F43">
         <v>23077.0</v>
@@ -2399,7 +2438,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I43">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J43">
         <v>0.0</v>
@@ -2411,7 +2450,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M43">
-        <v>18.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N43">
         <v>0.0</v>
@@ -2425,19 +2464,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B44">
-        <v>234076.0</v>
+        <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C44">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c s="1" r="D44">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E44">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c s="1" r="F44">
-        <v>23077.0</v>
+        <v>26631.0</v>
       </c>
       <c s="1" r="G44">
         <v>0.0</v>
@@ -2446,22 +2485,22 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I44">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="J44">
         <v>0.0</v>
       </c>
       <c s="1" r="K44">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="L44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M44">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="N44">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="O44">
         <v>0.0</v>
@@ -2475,13 +2514,13 @@
         <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C45">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c s="1" r="D45">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E45">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c s="1" r="F45">
         <v>26631.0</v>
@@ -2493,22 +2532,22 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I45">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J45">
         <v>0.0</v>
       </c>
       <c s="1" r="K45">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="L45">
         <v>1.0</v>
       </c>
       <c s="1" r="M45">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N45">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="O45">
         <v>0.0</v>
@@ -2519,19 +2558,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B46">
-        <v>234030.0</v>
+        <v>233912.0</v>
       </c>
       <c t="s" s="1" r="C46">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c s="1" r="D46">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E46">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c s="1" r="F46">
-        <v>26631.0</v>
+        <v>1124.0</v>
       </c>
       <c s="1" r="G46">
         <v>0.0</v>
@@ -2549,7 +2588,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L46">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M46">
         <v>0.0</v>
@@ -2566,19 +2605,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B47">
-        <v>233912.0</v>
+        <v>234085.0</v>
       </c>
       <c t="s" s="1" r="C47">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c s="1" r="D47">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E47">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c s="1" r="F47">
-        <v>1124.0</v>
+        <v>1333.0</v>
       </c>
       <c s="1" r="G47">
         <v>0.0</v>
@@ -2587,7 +2626,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I47">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="J47">
         <v>0.0</v>
@@ -2599,7 +2638,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M47">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="N47">
         <v>0.0</v>
@@ -2613,19 +2652,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B48">
-        <v>234085.0</v>
+        <v>233921.0</v>
       </c>
       <c t="s" s="1" r="C48">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c s="1" r="D48">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E48">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c s="1" r="F48">
-        <v>1333.0</v>
+        <v>27755.0</v>
       </c>
       <c s="1" r="G48">
         <v>0.0</v>
@@ -2634,7 +2673,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I48">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="J48">
         <v>0.0</v>
@@ -2643,10 +2682,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L48">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="M48">
-        <v>3.0</v>
+        <v>15.0</v>
       </c>
       <c s="1" r="N48">
         <v>0.0</v>
@@ -2660,19 +2699,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B49">
-        <v>233921.0</v>
+        <v>234155.0</v>
       </c>
       <c t="s" s="1" r="C49">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c s="1" r="D49">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E49">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c s="1" r="F49">
-        <v>27755.0</v>
+        <v>4933.0</v>
       </c>
       <c s="1" r="G49">
         <v>0.0</v>
@@ -2681,19 +2720,19 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I49">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J49">
         <v>0.0</v>
       </c>
       <c s="1" r="K49">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="L49">
         <v>2.0</v>
       </c>
       <c s="1" r="M49">
-        <v>15.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="N49">
         <v>0.0</v>
@@ -2707,19 +2746,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B50">
-        <v>234155.0</v>
+        <v>234164.0</v>
       </c>
       <c t="s" s="1" r="C50">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c s="1" r="D50">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E50">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c s="1" r="F50">
-        <v>4933.0</v>
+        <v>1961.0</v>
       </c>
       <c s="1" r="G50">
         <v>0.0</v>
@@ -2734,13 +2773,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="K50">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="L50">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M50">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
       <c s="1" r="N50">
         <v>0.0</v>
@@ -2754,19 +2793,16 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B51">
-        <v>234164.0</v>
+        <v>234137.0</v>
       </c>
       <c t="s" s="1" r="C51">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c s="1" r="D51">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E51">
-        <v>113</v>
-      </c>
-      <c s="1" r="F51">
-        <v>1961.0</v>
+        <v>114</v>
       </c>
       <c s="1" r="G51">
         <v>0.0</v>
@@ -2784,10 +2820,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L51">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M51">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N51">
         <v>0.0</v>
@@ -2801,16 +2837,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B52">
-        <v>234137.0</v>
+        <v>234173.0</v>
       </c>
       <c t="s" s="1" r="C52">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c s="1" r="D52">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E52">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c s="1" r="F52">
+        <v>1429.0</v>
       </c>
       <c s="1" r="G52">
         <v>0.0</v>
@@ -2819,7 +2858,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I52">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="J52">
         <v>0.0</v>
@@ -2845,19 +2884,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B53">
-        <v>234173.0</v>
+        <v>234207.0</v>
       </c>
       <c t="s" s="1" r="C53">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c s="1" r="D53">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E53">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c s="1" r="F53">
-        <v>1429.0</v>
+        <v>2137.0</v>
       </c>
       <c s="1" r="G53">
         <v>0.0</v>
@@ -2866,7 +2905,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I53">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J53">
         <v>0.0</v>
@@ -2892,19 +2931,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B54">
-        <v>234207.0</v>
+        <v>234359.0</v>
       </c>
       <c t="s" s="1" r="C54">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c s="1" r="D54">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E54">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c s="1" r="F54">
-        <v>2137.0</v>
+        <v>273.0</v>
       </c>
       <c s="1" r="G54">
         <v>0.0</v>
@@ -2931,53 +2970,6 @@
         <v>0.0</v>
       </c>
       <c s="1" r="O54">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c s="1" r="A55">
-        <v>2003.0</v>
-      </c>
-      <c s="1" r="B55">
-        <v>234359.0</v>
-      </c>
-      <c t="s" s="1" r="C55">
-        <v>120</v>
-      </c>
-      <c s="1" r="D55">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="1" r="E55">
-        <v>121</v>
-      </c>
-      <c s="1" r="F55">
-        <v>273.0</v>
-      </c>
-      <c s="1" r="G55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="I55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="J55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="K55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="L55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="M55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="N55">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="O55">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>